<commit_message>
Show SYMBOl instead of ENTREZID
</commit_message>
<xml_diff>
--- a/processed-data/04_gene_ontology/TableSxx_GO_KEGG.xlsx
+++ b/processed-data/04_gene_ontology/TableSxx_GO_KEGG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leocollado/Dropbox/Code/TREG_paper/processed-data/04_gene_ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF12020-C867-5A42-BDBD-2E939E0A032C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75ACD736-5AC0-8544-A9F3-3005B896AB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="40780" windowHeight="25440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -317,9 +317,6 @@
     <t>58/4501</t>
   </si>
   <si>
-    <t>10000/5894/2033</t>
-  </si>
-  <si>
     <t>hsa04630</t>
   </si>
   <si>
@@ -401,9 +398,6 @@
     <t>109/4501</t>
   </si>
   <si>
-    <t>10000/57492/5894</t>
-  </si>
-  <si>
     <t>hsa05167</t>
   </si>
   <si>
@@ -434,9 +428,6 @@
     <t>38/4501</t>
   </si>
   <si>
-    <t>10000/5894</t>
-  </si>
-  <si>
     <t>hsa04664</t>
   </si>
   <si>
@@ -455,9 +446,6 @@
     <t>44/4501</t>
   </si>
   <si>
-    <t>6310/2033</t>
-  </si>
-  <si>
     <t>hsa04917</t>
   </si>
   <si>
@@ -524,9 +512,6 @@
     <t>Long-term potentiation</t>
   </si>
   <si>
-    <t>5894/2033</t>
-  </si>
-  <si>
     <t>hsa05223</t>
   </si>
   <si>
@@ -629,9 +614,6 @@
     <t>68/4501</t>
   </si>
   <si>
-    <t>10000/2033</t>
-  </si>
-  <si>
     <t>hsa04012</t>
   </si>
   <si>
@@ -791,16 +773,34 @@
     <t>4/20</t>
   </si>
   <si>
-    <t>10000/5894/2033/2776</t>
-  </si>
-  <si>
-    <t>10000/5894/2033/23389</t>
-  </si>
-  <si>
     <t>3/20</t>
   </si>
   <si>
-    <t>10000/5894/2776</t>
+    <t>AKT3/RAF1/EP300</t>
+  </si>
+  <si>
+    <t>AKT3/ARID1B/RAF1</t>
+  </si>
+  <si>
+    <t>AKT3/RAF1</t>
+  </si>
+  <si>
+    <t>ATXN1/EP300</t>
+  </si>
+  <si>
+    <t>RAF1/EP300</t>
+  </si>
+  <si>
+    <t>AKT3/EP300</t>
+  </si>
+  <si>
+    <t>AKT3/RAF1/EP300/GNAQ</t>
+  </si>
+  <si>
+    <t>AKT3/RAF1/EP300/MED13L</t>
+  </si>
+  <si>
+    <t>AKT3/RAF1/GNAQ</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1190,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1940,12 +1940,12 @@
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>6.3909660113173226E-3</v>
       </c>
       <c r="I2" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J2">
         <v>3</v>
@@ -2014,16 +2014,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>100</v>
       </c>
       <c r="D3" t="s">
         <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3">
         <v>3.2094890005569181E-4</v>
@@ -2035,7 +2035,7 @@
         <v>6.3909660113173226E-3</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J3">
         <v>3</v>
@@ -2046,16 +2046,16 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
         <v>102</v>
-      </c>
-      <c r="C4" t="s">
-        <v>103</v>
       </c>
       <c r="D4" t="s">
         <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F4">
         <v>3.3583732282503891E-4</v>
@@ -2067,7 +2067,7 @@
         <v>6.3909660113173226E-3</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -2078,16 +2078,16 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
         <v>105</v>
-      </c>
-      <c r="C5" t="s">
-        <v>106</v>
       </c>
       <c r="D5" t="s">
         <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F5">
         <v>5.9313517594178486E-4</v>
@@ -2099,7 +2099,7 @@
         <v>6.3909660113173226E-3</v>
       </c>
       <c r="I5" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J5">
         <v>3</v>
@@ -2110,16 +2110,16 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
         <v>108</v>
-      </c>
-      <c r="C6" t="s">
-        <v>109</v>
       </c>
       <c r="D6" t="s">
         <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F6">
         <v>6.8465008999193044E-4</v>
@@ -2131,7 +2131,7 @@
         <v>6.3909660113173226E-3</v>
       </c>
       <c r="I6" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J6">
         <v>3</v>
@@ -2142,16 +2142,16 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" t="s">
         <v>111</v>
-      </c>
-      <c r="C7" t="s">
-        <v>112</v>
       </c>
       <c r="D7" t="s">
         <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F7">
         <v>7.3362060932061137E-4</v>
@@ -2163,7 +2163,7 @@
         <v>6.3909660113173226E-3</v>
       </c>
       <c r="I7" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J7">
         <v>3</v>
@@ -2174,16 +2174,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" t="s">
         <v>114</v>
-      </c>
-      <c r="C8" t="s">
-        <v>115</v>
       </c>
       <c r="D8" t="s">
         <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F8">
         <v>7.5892721384393199E-4</v>
@@ -2195,7 +2195,7 @@
         <v>6.3909660113173226E-3</v>
       </c>
       <c r="I8" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J8">
         <v>3</v>
@@ -2206,16 +2206,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" t="s">
         <v>117</v>
-      </c>
-      <c r="C9" t="s">
-        <v>118</v>
       </c>
       <c r="D9" t="s">
         <v>96</v>
       </c>
       <c r="E9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F9">
         <v>8.9387679537353975E-4</v>
@@ -2227,7 +2227,7 @@
         <v>6.586460597489241E-3</v>
       </c>
       <c r="I9" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J9">
         <v>3</v>
@@ -2238,16 +2238,16 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
         <v>120</v>
-      </c>
-      <c r="C10" t="s">
-        <v>121</v>
       </c>
       <c r="D10" t="s">
         <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F10">
         <v>1.207837867621072E-3</v>
@@ -2259,7 +2259,7 @@
         <v>7.9109848639508807E-3</v>
       </c>
       <c r="I10" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J10">
         <v>3</v>
@@ -2270,16 +2270,16 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
         <v>123</v>
-      </c>
-      <c r="C11" t="s">
-        <v>124</v>
       </c>
       <c r="D11" t="s">
         <v>96</v>
       </c>
       <c r="E11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F11">
         <v>1.4646538588284901E-3</v>
@@ -2291,7 +2291,7 @@
         <v>8.6337490625679435E-3</v>
       </c>
       <c r="I11" t="s">
-        <v>126</v>
+        <v>252</v>
       </c>
       <c r="J11">
         <v>3</v>
@@ -2302,16 +2302,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D12" t="s">
         <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F12">
         <v>1.710434149676804E-3</v>
@@ -2323,7 +2323,7 @@
         <v>9.1659629073589516E-3</v>
       </c>
       <c r="I12" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J12">
         <v>3</v>
@@ -2334,16 +2334,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
       </c>
       <c r="E13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F13">
         <v>2.5438387828822101E-3</v>
@@ -2355,7 +2355,7 @@
         <v>1.23205959692924E-2</v>
       </c>
       <c r="I13" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J13">
         <v>3</v>
@@ -2366,16 +2366,16 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" t="s">
         <v>134</v>
-      </c>
-      <c r="D14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" t="s">
-        <v>136</v>
       </c>
       <c r="F14">
         <v>2.9931309013443469E-3</v>
@@ -2387,7 +2387,7 @@
         <v>1.23205959692924E-2</v>
       </c>
       <c r="I14" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -2398,16 +2398,16 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F15">
         <v>3.8219132318697739E-3</v>
@@ -2419,7 +2419,7 @@
         <v>1.23205959692924E-2</v>
       </c>
       <c r="I15" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J15">
         <v>2</v>
@@ -2430,16 +2430,16 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F16">
         <v>3.9991594865121868E-3</v>
@@ -2451,7 +2451,7 @@
         <v>1.23205959692924E-2</v>
       </c>
       <c r="I16" t="s">
-        <v>144</v>
+        <v>254</v>
       </c>
       <c r="J16">
         <v>2</v>
@@ -2462,16 +2462,16 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F17">
         <v>3.9991594865121868E-3</v>
@@ -2483,7 +2483,7 @@
         <v>1.23205959692924E-2</v>
       </c>
       <c r="I17" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J17">
         <v>2</v>
@@ -2494,16 +2494,16 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F18">
         <v>3.9991594865121868E-3</v>
@@ -2515,7 +2515,7 @@
         <v>1.23205959692924E-2</v>
       </c>
       <c r="I18" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J18">
         <v>2</v>
@@ -2526,16 +2526,16 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C19" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F19">
         <v>3.9991594865121868E-3</v>
@@ -2547,7 +2547,7 @@
         <v>1.23205959692924E-2</v>
       </c>
       <c r="I19" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J19">
         <v>2</v>
@@ -2558,16 +2558,16 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F20">
         <v>3.9991594865121868E-3</v>
@@ -2579,7 +2579,7 @@
         <v>1.23205959692924E-2</v>
       </c>
       <c r="I20" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J20">
         <v>2</v>
@@ -2590,16 +2590,16 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F21">
         <v>4.1802022038670648E-3</v>
@@ -2611,7 +2611,7 @@
         <v>1.23205959692924E-2</v>
       </c>
       <c r="I21" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J21">
         <v>2</v>
@@ -2622,16 +2622,16 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C22" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E22" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F22">
         <v>4.7459665589361204E-3</v>
@@ -2643,7 +2643,7 @@
         <v>1.324186375906228E-2</v>
       </c>
       <c r="I22" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J22">
         <v>2</v>
@@ -2654,16 +2654,16 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C23" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E23" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F23">
         <v>4.9420527243643157E-3</v>
@@ -2675,7 +2675,7 @@
         <v>1.324186375906228E-2</v>
       </c>
       <c r="I23" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J23">
         <v>2</v>
@@ -2686,16 +2686,16 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E24" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F24">
         <v>6.1963113142063922E-3</v>
@@ -2707,7 +2707,7 @@
         <v>1.3986688595425111E-2</v>
       </c>
       <c r="I24" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J24">
         <v>2</v>
@@ -2718,16 +2718,16 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E25" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F25">
         <v>6.1963113142063922E-3</v>
@@ -2739,7 +2739,7 @@
         <v>1.3986688595425111E-2</v>
       </c>
       <c r="I25" t="s">
-        <v>167</v>
+        <v>255</v>
       </c>
       <c r="J25">
         <v>2</v>
@@ -2750,16 +2750,16 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C26" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E26" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F26">
         <v>6.1963113142063922E-3</v>
@@ -2771,7 +2771,7 @@
         <v>1.3986688595425111E-2</v>
       </c>
       <c r="I26" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J26">
         <v>2</v>
@@ -2782,16 +2782,16 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C27" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E27" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F27">
         <v>6.4181804934153163E-3</v>
@@ -2803,7 +2803,7 @@
         <v>1.3986688595425111E-2</v>
       </c>
       <c r="I27" t="s">
-        <v>167</v>
+        <v>255</v>
       </c>
       <c r="J27">
         <v>2</v>
@@ -2814,16 +2814,16 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C28" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E28" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F28">
         <v>6.4181804934153163E-3</v>
@@ -2835,7 +2835,7 @@
         <v>1.3986688595425111E-2</v>
       </c>
       <c r="I28" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J28">
         <v>2</v>
@@ -2846,16 +2846,16 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C29" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E29" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F29">
         <v>6.6436770828269256E-3</v>
@@ -2867,7 +2867,7 @@
         <v>1.3986688595425111E-2</v>
       </c>
       <c r="I29" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J29">
         <v>2</v>
@@ -2878,16 +2878,16 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C30" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E30" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F30">
         <v>7.1054970509678971E-3</v>
@@ -2899,7 +2899,7 @@
         <v>1.444311560269337E-2</v>
       </c>
       <c r="I30" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J30">
         <v>2</v>
@@ -2910,16 +2910,16 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C31" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E31" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F31">
         <v>7.5816606698088417E-3</v>
@@ -2931,7 +2931,7 @@
         <v>1.4869611214763869E-2</v>
       </c>
       <c r="I31" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J31">
         <v>2</v>
@@ -2942,16 +2942,16 @@
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C32" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D32" t="s">
         <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F32">
         <v>8.2264373217099309E-3</v>
@@ -2963,7 +2963,7 @@
         <v>1.4869611214763869E-2</v>
       </c>
       <c r="I32" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J32">
         <v>3</v>
@@ -2974,16 +2974,16 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C33" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E33" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F33">
         <v>8.3225599279475957E-3</v>
@@ -2995,7 +2995,7 @@
         <v>1.4869611214763869E-2</v>
       </c>
       <c r="I33" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J33">
         <v>2</v>
@@ -3006,16 +3006,16 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C34" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F34">
         <v>8.5765793256584455E-3</v>
@@ -3027,7 +3027,7 @@
         <v>1.4869611214763869E-2</v>
       </c>
       <c r="I34" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J34">
         <v>2</v>
@@ -3038,16 +3038,16 @@
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C35" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F35">
         <v>8.5765793256584455E-3</v>
@@ -3059,7 +3059,7 @@
         <v>1.4869611214763869E-2</v>
       </c>
       <c r="I35" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J35">
         <v>2</v>
@@ -3070,16 +3070,16 @@
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C36" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D36" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E36" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F36">
         <v>9.0951159205698382E-3</v>
@@ -3091,7 +3091,7 @@
         <v>1.4892587472278101E-2</v>
       </c>
       <c r="I36" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J36">
         <v>2</v>
@@ -3102,16 +3102,16 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C37" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E37" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F37">
         <v>9.0951159205698382E-3</v>
@@ -3123,7 +3123,7 @@
         <v>1.4892587472278101E-2</v>
       </c>
       <c r="I37" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J37">
         <v>2</v>
@@ -3134,16 +3134,16 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C38" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E38" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F38">
         <v>9.3596060103524319E-3</v>
@@ -3155,7 +3155,7 @@
         <v>1.491146334508496E-2</v>
       </c>
       <c r="I38" t="s">
-        <v>202</v>
+        <v>256</v>
       </c>
       <c r="J38">
         <v>2</v>
@@ -3166,16 +3166,16 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C39" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E39" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="F39">
         <v>9.6275592781289721E-3</v>
@@ -3187,7 +3187,7 @@
         <v>1.493471799377348E-2</v>
       </c>
       <c r="I39" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J39">
         <v>2</v>
@@ -3198,16 +3198,16 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C40" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E40" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F40">
         <v>1.0173801493485681E-2</v>
@@ -3219,7 +3219,7 @@
         <v>1.537740576613221E-2</v>
       </c>
       <c r="I40" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J40">
         <v>2</v>
@@ -3230,16 +3230,16 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C41" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E41" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F41">
         <v>1.101880291969703E-2</v>
@@ -3251,7 +3251,7 @@
         <v>1.5464986553960751E-2</v>
       </c>
       <c r="I41" t="s">
-        <v>202</v>
+        <v>256</v>
       </c>
       <c r="J41">
         <v>2</v>
@@ -3262,16 +3262,16 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C42" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E42" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F42">
         <v>1.101880291969703E-2</v>
@@ -3283,7 +3283,7 @@
         <v>1.5464986553960751E-2</v>
       </c>
       <c r="I42" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J42">
         <v>2</v>
@@ -3294,16 +3294,16 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C43" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E43" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F43">
         <v>1.101880291969703E-2</v>
@@ -3315,7 +3315,7 @@
         <v>1.5464986553960751E-2</v>
       </c>
       <c r="I43" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J43">
         <v>2</v>
@@ -3326,16 +3326,16 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C44" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E44" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F44">
         <v>1.1894250071784501E-2</v>
@@ -3347,7 +3347,7 @@
         <v>1.5934880478945739E-2</v>
       </c>
       <c r="I44" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J44">
         <v>2</v>
@@ -3358,16 +3358,16 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C45" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E45" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F45">
         <v>1.1894250071784501E-2</v>
@@ -3379,7 +3379,7 @@
         <v>1.5934880478945739E-2</v>
       </c>
       <c r="I45" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J45">
         <v>2</v>
@@ -3390,16 +3390,16 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C46" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E46" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F46">
         <v>1.2192769624421999E-2</v>
@@ -3411,7 +3411,7 @@
         <v>1.5971815180529401E-2</v>
       </c>
       <c r="I46" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J46">
         <v>2</v>
@@ -3422,16 +3422,16 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C47" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D47" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E47" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F47">
         <v>1.24946191017462E-2</v>
@@ -3443,7 +3443,7 @@
         <v>1.601141120589903E-2</v>
       </c>
       <c r="I47" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J47">
         <v>2</v>
@@ -3454,16 +3454,16 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C48" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D48" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E48" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F48">
         <v>1.3735053788930279E-2</v>
@@ -3475,7 +3475,7 @@
         <v>1.7226495233596768E-2</v>
       </c>
       <c r="I48" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J48">
         <v>2</v>
@@ -3486,16 +3486,16 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C49" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D49" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F49">
         <v>1.4053356318172691E-2</v>
@@ -3507,7 +3507,7 @@
         <v>1.7258507759159439E-2</v>
       </c>
       <c r="I49" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J49">
         <v>2</v>
@@ -3518,16 +3518,16 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C50" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D50" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F50">
         <v>1.502772123396454E-2</v>
@@ -3539,7 +3539,7 @@
         <v>1.807846163484457E-2</v>
       </c>
       <c r="I50" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J50">
         <v>2</v>
@@ -3550,16 +3550,16 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C51" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D51" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E51" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F51">
         <v>1.5693383122887369E-2</v>
@@ -3571,7 +3571,7 @@
         <v>1.8501672734351431E-2</v>
       </c>
       <c r="I51" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J51">
         <v>2</v>
@@ -3582,16 +3582,16 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C52" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D52" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E52" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="F52">
         <v>1.6371793274233409E-2</v>
@@ -3603,7 +3603,7 @@
         <v>1.8923022153912721E-2</v>
       </c>
       <c r="I52" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J52">
         <v>2</v>
@@ -3614,16 +3614,16 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C53" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D53" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F53">
         <v>1.6715746973763639E-2</v>
@@ -3635,7 +3635,7 @@
         <v>1.8949024909529631E-2</v>
       </c>
       <c r="I53" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J53">
         <v>2</v>
@@ -3646,16 +3646,16 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C54" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D54" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E54" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F54">
         <v>1.9579668734752639E-2</v>
@@ -3667,7 +3667,7 @@
         <v>2.1396189403842181E-2</v>
       </c>
       <c r="I54" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J54">
         <v>2</v>
@@ -3678,16 +3678,16 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C55" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E55" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="F55">
         <v>1.995150655980639E-2</v>
@@ -3699,7 +3699,7 @@
         <v>2.1396189403842181E-2</v>
       </c>
       <c r="I55" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J55">
         <v>2</v>
@@ -3710,16 +3710,16 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C56" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F56">
         <v>2.0326379933650069E-2</v>
@@ -3731,7 +3731,7 @@
         <v>2.1396189403842181E-2</v>
       </c>
       <c r="I56" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J56">
         <v>2</v>
@@ -3742,16 +3742,16 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C57" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="D57" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F57">
         <v>2.0326379933650069E-2</v>
@@ -3763,7 +3763,7 @@
         <v>2.1396189403842181E-2</v>
       </c>
       <c r="I57" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J57">
         <v>2</v>
@@ -3774,16 +3774,16 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C58" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D58" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E58" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F58">
         <v>2.1855980897004589E-2</v>
@@ -3795,7 +3795,7 @@
         <v>2.2602676458582771E-2</v>
       </c>
       <c r="I58" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="J58">
         <v>2</v>
@@ -3806,16 +3806,16 @@
         <v>29</v>
       </c>
       <c r="B59" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" t="s">
         <v>108</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
+        <v>249</v>
+      </c>
+      <c r="E59" t="s">
         <v>109</v>
-      </c>
-      <c r="D59" t="s">
-        <v>255</v>
-      </c>
-      <c r="E59" t="s">
-        <v>110</v>
       </c>
       <c r="F59">
         <v>4.3552446891269048E-4</v>
@@ -3827,7 +3827,7 @@
         <v>2.7251455003829399E-2</v>
       </c>
       <c r="I59" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J59">
         <v>4</v>
@@ -3838,16 +3838,16 @@
         <v>29</v>
       </c>
       <c r="B60" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" t="s">
         <v>117</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
+        <v>249</v>
+      </c>
+      <c r="E60" t="s">
         <v>118</v>
-      </c>
-      <c r="D60" t="s">
-        <v>255</v>
-      </c>
-      <c r="E60" t="s">
-        <v>119</v>
       </c>
       <c r="F60">
         <v>6.1640195841995054E-4</v>
@@ -3859,7 +3859,7 @@
         <v>2.7251455003829399E-2</v>
       </c>
       <c r="I60" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="J60">
         <v>4</v>
@@ -3870,16 +3870,16 @@
         <v>29</v>
       </c>
       <c r="B61" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C61" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D61" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E61" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F61">
         <v>9.4545149818110632E-4</v>

</xml_diff>